<commit_message>
improve xml et multithread
xml : gestion de tag en doublons par ajou de sub tag
multithread : il arrivait qu'un thread se bloque
</commit_message>
<xml_diff>
--- a/Excel/queryHelper/saved_SGE.xlsx
+++ b/Excel/queryHelper/saved_SGE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,17 @@
     <sheet name="DEM77" sheetId="43" r:id="rId6"/>
     <sheet name="DEM77_RES" sheetId="44" r:id="rId7"/>
     <sheet name="Vol prs TRV" sheetId="45" r:id="rId8"/>
-    <sheet name="M021" sheetId="47" r:id="rId9"/>
+    <sheet name="M021" sheetId="51" r:id="rId9"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId10"/>
   </externalReferences>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="141">
   <si>
     <t/>
   </si>
@@ -692,10 +692,10 @@
     <t>Cellule copiée dans le presse-papier</t>
   </si>
   <si>
-    <t>15/09/2020</t>
-  </si>
-  <si>
-    <t>SELECT COUNT(1) as VOLUMETRIE, PRS_OPTION, ETAT_EXTERNE FROM
+    <t>01/01/2020</t>
+  </si>
+  <si>
+    <t>SELECT TO_CHAR(DATE_DEMANDE, 'YYYY/MM/DD') as DATE_VOL, COUNT(1) as VOLUMETRIE, PRS_OPTION, FOURNISSEUR, ETAT_EXTERNE FROM
 (
 SELECT DISTINCT dem.AFF_T_DISCO as AFFAIRE, dem.DEM_ID_PRM as POINT, nat.NAT_C_PRESTATION as PRESTATION, nat.NAT_C_SOUS_TYPE as PRS_OPTION, DECODE(dem.DEM_K_CATEGORIE, '1', 'PRO', '2', 'PART') as CAT_CLIENT, frn.FRN_T_ACTEUR as FOURNISSEUR, dem.DEM_R_STATUT as STATUT, ee.EST_T_ETAT as ETAT_EXTERNE, ei.EST_T_ETAT as ETAT_INTERNE, dem.DEM_D_DEMANDE as DATE_DEMANDE, dem.DEM_D_EFFET as DATE_EFFET, DECODE(dem.DEM_K_MODALITE_RDV, '1', 'DIS', '2', 'FRN') as MOD_RDV, dem.DEM_R_MEDIA_RECEPTION as MEDIA, mai.MAI_T_REGION as REGION, mai.MAI_T_TERRITOIRE as TERRITOIRE, dem.DEM_B_IS_SGEL as SGEL, dem.DEM_B_IS_GINKO as GINKO
 FROM SUIVI.DEMANDE dem
@@ -706,9 +706,10 @@
 LEFT JOIN SUIVI.MAILLE mai ON mai.MAI_ID = dem.DEM_K_MAI
 WHERE 1=1
 AND nat.NAT_C_PRESTATION IN ('M021')
-AND dem.DEM_D_DEMANDE &gt;= TO_DATE('15/09/2020', 'DD/MM/YYYY')
+AND dem.DEM_D_DEMANDE &gt;= TO_DATE('01/01/2020', 'DD/MM/YYYY')
+ORDER BY dem.DEM_D_DEMANDE
 )
-GROUP BY PRS_OPTION, ETAT_EXTERNE
+GROUP BY PRS_OPTION, FOURNISSEUR, ETAT_EXTERNE, TO_CHAR(DATE_DEMANDE, 'YYYY/MM/DD')
 ORDER BY 1 DESC
 ;</t>
   </si>
@@ -9906,11 +9907,11 @@
       <c r="E8" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>0</v>
+      <c r="F8" s="71" t="s">
+        <v>82</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="2"/>
@@ -10328,10 +10329,12 @@
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="47" t="s">
+      <c r="J20" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="48"/>
+      <c r="K20" s="73" t="s">
+        <v>96</v>
+      </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="40" t="s">
@@ -10362,10 +10365,10 @@
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="47" t="s">
+      <c r="J21" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="50" t="s">
+      <c r="K21" s="74" t="s">
         <v>38</v>
       </c>
       <c r="L21" s="1"/>
@@ -10398,10 +10401,10 @@
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="47" t="s">
+      <c r="J22" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="K22" s="52" t="s">
+      <c r="K22" s="75" t="s">
         <v>71</v>
       </c>
       <c r="L22" s="1"/>

</xml_diff>